<commit_message>
Able to print a view of the student id's
</commit_message>
<xml_diff>
--- a/files/students.xlsx
+++ b/files/students.xlsx
@@ -20,30 +20,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Student Names</t>
   </si>
   <si>
-    <t xml:space="preserve">Richy Truitt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cortney Jordan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chris Truitt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jackie Truitt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bill Zingler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dylan Zingler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Noah Zingler</t>
+    <t xml:space="preserve">Adewonuloa Adeyemi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kwaku Appiah-Kesse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Londynn Atkinson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeno Ban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">William Bell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bella Cooper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leyver Fajardo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carlos Fiallos-Lopez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anthony Gibson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaiden Hill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haiden Hodgson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zach Mansel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parker McCormick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samantha Meija-Benitez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Margaret Oghomienor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin Ramsdell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anaiah Robinson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Johnathan Saavadra-Saavadra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abigail Schurman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jontae Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chloe St. Louis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tristen Culbruth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamari Meye</t>
   </si>
 </sst>
 </file>
@@ -58,6 +106,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -75,12 +124,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,9 +172,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -131,6 +194,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -139,56 +262,136 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>